<commit_message>
adding new gdp data table
</commit_message>
<xml_diff>
--- a/Notebooks/Angel/excel_charts/gdp_excel_charts_total.xlsx
+++ b/Notebooks/Angel/excel_charts/gdp_excel_charts_total.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5bb19dd04e3b7a9/Documents/GitHub/Global_Energy_Project/Notebooks/Angel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaq3\OneDrive\Documents\GitHub\Global_Energy_Project\Notebooks\Angel\excel_charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{04035CA6-6308-45AB-9BEE-5CF936A468AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0A2B3FE5-9B2C-4929-B9D0-9C56C7D16FC4}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{04035CA6-6308-45AB-9BEE-5CF936A468AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{97222069-D023-4F32-9C69-F15F3E9A9A41}"/>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="-13620" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1198,151 +1198,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -1350,153 +1290,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$52</c:f>
+              <c:f>Sheet1!$B$4:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>6706873292.2517996</c:v>
+                  <c:v>66442468040.323997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6664236463.7439003</c:v>
+                  <c:v>63980718012.218002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7565752327.9068003</c:v>
+                  <c:v>58222866436.445999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8004462821.2784004</c:v>
+                  <c:v>55893956971.064003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8279435516.0474997</c:v>
+                  <c:v>49295163815.666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9094086150.7007999</c:v>
+                  <c:v>44514811692.658997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10160101394.666</c:v>
+                  <c:v>42215957228.322998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9762577513.1532001</c:v>
+                  <c:v>42936704451.253998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10415509120.032</c:v>
+                  <c:v>35086807903.407997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11047500636.572001</c:v>
+                  <c:v>40803806293.120003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11454716518.083</c:v>
+                  <c:v>45720146034.627998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11666808115.281</c:v>
+                  <c:v>50776369593.107002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12497595052.781</c:v>
+                  <c:v>52250290430.009003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13066657984.997</c:v>
+                  <c:v>51459651854.557999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14025818301.837999</c:v>
+                  <c:v>52054778985.733002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15133629918.379999</c:v>
+                  <c:v>51799979961.103996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15853140799.039</c:v>
+                  <c:v>53248749121.992996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16246829838.121</c:v>
+                  <c:v>53884648662.874001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16142503388.804001</c:v>
+                  <c:v>57006184227.819</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16842521804.372999</c:v>
+                  <c:v>57945664001.514999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18700051593.625</c:v>
+                  <c:v>51004299298.551003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19750810853.791</c:v>
+                  <c:v>58180627642.765999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21782327889.522999</c:v>
+                  <c:v>57484959421.547997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21992260805.82</c:v>
+                  <c:v>60087433894.948997</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22456588252.125999</c:v>
+                  <c:v>60998034780.926003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23289320118.015999</c:v>
+                  <c:v>62754805353.154999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>22818443161.257</c:v>
+                  <c:v>64843098747.899002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22168065968.299</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>24712972224.577</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>23351032499.226002</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>24255768993.848999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>23647756556.93</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>27043184943.029999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>28809288119.507999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>28507940776.832001</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>31862757398.654999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>34328899942.133999</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>35091485243.765999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>27949235421.088001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>30078539446.521</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>31918418894.811001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>33106636958.527</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>34649110324.593002</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>36547017215.188004</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>38523380400.382004</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>40304054184.188004</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>41995259096.741997</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>43329852262.586998</c:v>
+                  <c:v>65616047808.931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1532,151 +1412,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -1684,153 +1504,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$52</c:f>
+              <c:f>Sheet1!$C$4:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>130869362668.7</c:v>
+                  <c:v>472689604063.90002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151066079936.64999</c:v>
+                  <c:v>445748690065.41998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>171573485728.35001</c:v>
+                  <c:v>365915592345.45001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>189838035760.06</c:v>
+                  <c:v>313107191782.65997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>190709422649.79999</c:v>
+                  <c:v>250375859544.44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>169378552430.70001</c:v>
+                  <c:v>241515372824.42001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>192630258142.47</c:v>
+                  <c:v>234944190934.87</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>178637697264.97</c:v>
+                  <c:v>239195246942.70001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>129411124067.77</c:v>
+                  <c:v>227256022870.07999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>101874260383.45</c:v>
+                  <c:v>249766862085.98001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40370031993.899002</c:v>
+                  <c:v>277715907823.65997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43445828678.880997</c:v>
+                  <c:v>291077805139.98999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84887644321.947006</c:v>
+                  <c:v>302191738520.89001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87401817783.488998</c:v>
+                  <c:v>327319754016.82001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>73621880277.098007</c:v>
+                  <c:v>359962969062.09998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74708834434.481003</c:v>
+                  <c:v>370203498365.26001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>65952793048.623001</c:v>
+                  <c:v>380397538207.01001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>75010824596.966995</c:v>
+                  <c:v>390286837986.44</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>80091520051.707993</c:v>
+                  <c:v>387482512094.17999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>85062716858.738007</c:v>
+                  <c:v>352138362390.67999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>102317396486.14999</c:v>
+                  <c:v>377688222229.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>116965914532.11</c:v>
+                  <c:v>394282114694.96002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>117688256239.27</c:v>
+                  <c:v>406528942968.38</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>122425085663.24001</c:v>
+                  <c:v>406991912729.28003</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>118009034674.74001</c:v>
+                  <c:v>408178729802.64001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>119755174269.34</c:v>
+                  <c:v>396458190565.85999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>121664429935.45</c:v>
+                  <c:v>397044320119.84003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>120357940237.16</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>122113168268.84</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>119652667423.75</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>130216122049.99001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>123393065487.36</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>130797047476.2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>147227540327.5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>152148018407.07999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>156656490758.73999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>164353668794.04001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>168052911727.89999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>169828801821.12</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>169742495883.82999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>181572240871.29001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>183846079410.39999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>145820599118.47</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>140814434654.04001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>149861413054.53</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>152391762722.35001</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>199427095834.62</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>205884468894.5</c:v>
+                  <c:v>398920728220.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1866,151 +1626,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -2018,153 +1718,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$52</c:f>
+              <c:f>Sheet1!$D$4:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>3681719617.8639998</c:v>
+                  <c:v>244410080985.98001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4275664365.8361001</c:v>
+                  <c:v>230483190942.89001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4996882988.3734999</c:v>
+                  <c:v>189201173921.89001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5913623795.026</c:v>
+                  <c:v>161893772033</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6877400598.8006001</c:v>
+                  <c:v>129467269908.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7440910289.8113003</c:v>
+                  <c:v>124873094669.96001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9675581290.3334999</c:v>
+                  <c:v>121474291431.78999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10157008554.993999</c:v>
+                  <c:v>123711873318.17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9095470659.1620007</c:v>
+                  <c:v>117465179459.12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7923259828.9252996</c:v>
+                  <c:v>129134172445.12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8898103926.1403008</c:v>
+                  <c:v>143772840067.81</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9612866627.5041008</c:v>
+                  <c:v>150178092612.64999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9192309476.7660999</c:v>
+                  <c:v>156360353117.95001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10286126978.466</c:v>
+                  <c:v>170119080064.41</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11549642979.587</c:v>
+                  <c:v>183818435630.41</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11306162523.896</c:v>
+                  <c:v>191974881733.48001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10587710724.719</c:v>
+                  <c:v>204591607128.85001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11764532927.223</c:v>
+                  <c:v>219981762251.89999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12006168834.006001</c:v>
+                  <c:v>215313223774.62</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12432324839.715</c:v>
+                  <c:v>183843231426.53</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15928841990.087999</c:v>
+                  <c:v>199669508795.01001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19303859407.09</c:v>
+                  <c:v>212213416439.89001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19127970072.530998</c:v>
+                  <c:v>221902498582.56</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18126387835.278</c:v>
+                  <c:v>223483559630.35999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>18729448809.678001</c:v>
+                  <c:v>225159739561.07999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18727221492.556999</c:v>
+                  <c:v>214740225530.82999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>21436323507.366001</c:v>
+                  <c:v>217206986056.67001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24378158925.900002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>23516239059.049</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>25973246221.300999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>28961106686.272999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32473612459.000999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>36793202261.731003</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>40381954667.922997</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>41907390030.185997</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>46309416806.348999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>49980505769.668999</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>50968211138.001999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>52556105253.031998</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>56816724302.574997</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>62781599464.891998</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>66327162530.347</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>63623361867.805</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>60282351660.946999</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>65096974759.447998</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>62076760507.538002</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>66333642656.197998</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>69855332020.781006</c:v>
+                  <c:v>217402467511.79001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2200,151 +1840,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -2352,153 +1932,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$52</c:f>
+              <c:f>Sheet1!$E$4:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>8726084495.9743996</c:v>
+                  <c:v>120208506407.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9567596236.1576004</c:v>
+                  <c:v>105787427091.14999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10213449415.110001</c:v>
+                  <c:v>70876590787.927994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13877912922.976999</c:v>
+                  <c:v>65206446180.060997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15110377374.108999</c:v>
+                  <c:v>52817228107.271004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16866943563.929001</c:v>
+                  <c:v>48063679154.410004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28899671977.523998</c:v>
+                  <c:v>39993840931.055</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23488383409.096001</c:v>
+                  <c:v>37818812404.108002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29283239963.227001</c:v>
+                  <c:v>35437867065.652</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22513342054.650002</c:v>
+                  <c:v>37546780242.907997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22015522625.543999</c:v>
+                  <c:v>44076146673.744003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17843013160.507999</c:v>
+                  <c:v>48439690014.873001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19860970867.632999</c:v>
+                  <c:v>49795994099.521004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24351196082.709999</c:v>
+                  <c:v>56097983872.718002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19697622719.338001</c:v>
+                  <c:v>61648136967.953003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18142148653.493999</c:v>
+                  <c:v>67944479297.449997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20605246319.488998</c:v>
+                  <c:v>76621861523.875</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19452878302.650002</c:v>
+                  <c:v>86588899388.774002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12777456062.875</c:v>
+                  <c:v>96177536374.621002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12717873330.231001</c:v>
+                  <c:v>82037511049.380997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13102966279.813</c:v>
+                  <c:v>85673914628.449005</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16945338972.913</c:v>
+                  <c:v>92222350752.942993</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17890497335.757999</c:v>
+                  <c:v>95757707353.110992</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17917384274.603001</c:v>
+                  <c:v>94279204003.546005</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17670310296.113998</c:v>
+                  <c:v>94042783671.820999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>16541373499.302</c:v>
+                  <c:v>93500769315.306</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18543152041.021</c:v>
+                  <c:v>92435140348.725006</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15778984005.614</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>14368083217.231001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>17378782558.362</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>18798214805.714001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>21784860540.119999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>26280484467.533001</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>26044312518.067001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>26061352650.664001</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>26735374735.150002</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>25933872763.188999</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>32392031992.330002</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>36573667508.332001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>34835208456.039001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>35539431280.113998</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>37347333486.434998</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>36142951484.542999</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>32801140731.603001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>32501474897.666</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>26974113590.859001</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>23451245231.005001</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>23728986935.409</c:v>
+                  <c:v>93282461233.804001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2534,151 +2054,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -2686,153 +2146,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$52</c:f>
+              <c:f>Sheet1!$F$4:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>7601603928.4404001</c:v>
+                  <c:v>138870979271.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9104786453.3546009</c:v>
+                  <c:v>134178717570.94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12313009899.584</c:v>
+                  <c:v>127705302371.55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10919719300.884001</c:v>
+                  <c:v>123746451395.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13351248562.684999</c:v>
+                  <c:v>123622698881.08</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16753016292.819</c:v>
+                  <c:v>118554187644.11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19466987563.068001</c:v>
+                  <c:v>120978939301.61</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18576602489.641998</c:v>
+                  <c:v>127447024761.91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19030312004.263</c:v>
+                  <c:v>119302300380.28</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16823783003.447001</c:v>
+                  <c:v>117008165851.37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14597828004.705</c:v>
+                  <c:v>131265839803.42999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13605829203.864</c:v>
+                  <c:v>136430896030.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13967818868.943001</c:v>
+                  <c:v>147614942968.70001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19922731600.384998</c:v>
+                  <c:v>166571619299.01001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22872423665.710999</c:v>
+                  <c:v>183267914028.20001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21763426612</c:v>
+                  <c:v>200034461372.57001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19418524832.323002</c:v>
+                  <c:v>227714516562.48999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19356561824.5</c:v>
+                  <c:v>254574139947.89999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18730113088.596001</c:v>
+                  <c:v>279706029031.77002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20374859395.463001</c:v>
+                  <c:v>262143312785.73999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21710330971.335999</c:v>
+                  <c:v>277439640369.34003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24414353220.534</c:v>
+                  <c:v>286733472500.53998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>26010424933.701</c:v>
+                  <c:v>296787766017.81</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24203137590.994999</c:v>
+                  <c:v>297014474557.53998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23373337186.005001</c:v>
+                  <c:v>306893856324.32001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23157068739.518002</c:v>
+                  <c:v>297855130196.84003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27016329930.327999</c:v>
+                  <c:v>295124767825.01001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27782377957.234001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28866204659.923</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29223060271.693001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30957156988.033001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>33610506477.310001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>36312507285.532997</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>39831520283.874001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44331626483.068001</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>48236277298.360001</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>50168783512.267998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>53392765615.635002</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>51025727698.656998</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>53388893157.902</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>57236483271.041</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>59447581734.342003</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>54562270321.863998</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>54356633078.899002</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>54624034899.174004</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>51300514902.539001</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>54494992922.711998</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>57077832347.925003</c:v>
+                  <c:v>302564293485.40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2868,151 +2268,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -3020,153 +2360,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$52</c:f>
+              <c:f>Sheet1!$G$4:$G$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>3637367998.9530001</c:v>
+                  <c:v>138311918804.81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4108961583.9742999</c:v>
+                  <c:v>130339108450.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5977509748.3056002</c:v>
+                  <c:v>109377229559.28999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7074240647.9315996</c:v>
+                  <c:v>87343204484.615997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9453922820.1963997</c:v>
+                  <c:v>73272571212.809998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11501013469.243</c:v>
+                  <c:v>71413488571.852005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12162589171.452</c:v>
+                  <c:v>68082061692.324997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12273055315.690001</c:v>
+                  <c:v>66848215964.595001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11417356770.43</c:v>
+                  <c:v>64918823354.265999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12505244763.973</c:v>
+                  <c:v>71107805680.613007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12679758813.695999</c:v>
+                  <c:v>75485396546.813004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10329174013.35</c:v>
+                  <c:v>79697833873.326996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10804024033.627001</c:v>
+                  <c:v>84245602008.166</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12487165933.76</c:v>
+                  <c:v>90351992200.259995</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12721152035.978001</c:v>
+                  <c:v>95688374675.820999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12729910723.907</c:v>
+                  <c:v>101352116760.17999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11025559885.535</c:v>
+                  <c:v>111207460124.37</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9023554021.1506996</c:v>
+                  <c:v>116594715069.25999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8417351754.6497002</c:v>
+                  <c:v>122705903050.72</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9280262238.3185997</c:v>
+                  <c:v>112183029691.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10143891208.299</c:v>
+                  <c:v>118329718079.89999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10290708658.847</c:v>
+                  <c:v>125983276335.22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10567515528.224001</c:v>
+                  <c:v>131017664115.81</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12343139898.517</c:v>
+                  <c:v>130777232909.61</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13614175277.226999</c:v>
+                  <c:v>135148628829.33</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14995295525.047001</c:v>
+                  <c:v>131269445323.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17117711323.284</c:v>
+                  <c:v>129992581888.71001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>17458898678.555</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>17969193311.271999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>20441646070.469002</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>21543621547.629002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>22960017997.910999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>24306456479.300999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>28838645423.532001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>31307076058.085999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>33696064528.417</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36794303384.941002</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>40546640112.466003</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44340960941.999001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>47516688169.103996</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>50071734330.658997</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>51464646284.294998</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>54431392359.763</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>54953414699.585999</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>55812510146.769997</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>52421356725.643997</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>55914526209.014</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>59862466928.68</c:v>
+                  <c:v>133285382801.49001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3204,151 +2484,91 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$52</c:f>
+              <c:f>Sheet1!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1970</c:v>
+                  <c:v>1990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1971</c:v>
+                  <c:v>1991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1972</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1973</c:v>
+                  <c:v>1993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1974</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1975</c:v>
+                  <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1976</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1977</c:v>
+                  <c:v>1997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1978</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1979</c:v>
+                  <c:v>1999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1980</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1981</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1982</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1983</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1984</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1985</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1987</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1988</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1989</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1990</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1991</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1993</c:v>
+                  <c:v>2013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1994</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1995</c:v>
+                  <c:v>2015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1996</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
@@ -3356,153 +2576,93 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$4:$H$52</c:f>
+              <c:f>Sheet1!$H$4:$H$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>40225319701.610001</c:v>
+                  <c:v>302048246050.73999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45908857962.728996</c:v>
+                  <c:v>304856274888.58002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52922190211.123001</c:v>
+                  <c:v>287262862205.26001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54714940452.987</c:v>
+                  <c:v>292458199671.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79265027120.636993</c:v>
+                  <c:v>262983800484</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91758968546.654999</c:v>
+                  <c:v>257192222909.42999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>104488629523.25</c:v>
+                  <c:v>258981072463.39001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112249701910.16</c:v>
+                  <c:v>262048918509.98001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>118394669901.39999</c:v>
+                  <c:v>261875364882.35999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>127491074116.66</c:v>
+                  <c:v>269753960628.45001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>122777513770.83</c:v>
+                  <c:v>276320916932.79999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110394567110.81</c:v>
+                  <c:v>282234065363.02002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105510878649.14999</c:v>
+                  <c:v>290275229810.28003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>104518243763.2</c:v>
+                  <c:v>300096376842.32001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97512747365.591995</c:v>
+                  <c:v>306524184779.96002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>102970708559.57001</c:v>
+                  <c:v>324692050255.54999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>86676187228.852997</c:v>
+                  <c:v>350601290430.21997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>78228615550.632004</c:v>
+                  <c:v>396538405306.84003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>66711191333.992996</c:v>
+                  <c:v>424386984462.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>70113675035.927994</c:v>
+                  <c:v>412578856136.28003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>77622235255.556</c:v>
+                  <c:v>422278449043.40002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>85335594342.412994</c:v>
+                  <c:v>425820046232.83002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>87848056784.927994</c:v>
+                  <c:v>445516678133.90002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>89777048759.035004</c:v>
+                  <c:v>466887563323.01001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>92359548579.569</c:v>
+                  <c:v>466119863669.54999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>94544695875.408997</c:v>
+                  <c:v>455804039892.94</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>90663712369.509003</c:v>
+                  <c:v>454537198358.35999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>95000099341.766006</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>96634635397.994003</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>97913097875.828003</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>97961614915.186996</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>101404774965.24001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>107883664846.96001</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>110348628264.67999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>114845850049.77</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>122199102065.78</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>131992755410.60001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>145172866525.81</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>140947416923.17001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>137675037259.76999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>143826440306.85999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>150338525088.13</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>157064156080.22</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>163033208188.29999</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>165873074327.03</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>166580315082.38</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>169334026580.57001</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>175066490614.57001</c:v>
+                  <c:v>462840969890.66998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26090,8 +25250,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A3:H52" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:H32" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
       <items count="45">
@@ -26207,67 +25367,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="49">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
+  <rowItems count="29">
     <i>
       <x v="20"/>
     </i>
@@ -26383,7 +25483,7 @@
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="0" item="15" hier="-1"/>
+    <pageField fld="0" item="29" hier="-1"/>
   </pageFields>
   <dataFields count="7">
     <dataField name="Sum of Agriculture" fld="2" baseField="0" baseItem="0"/>
@@ -26768,22 +25868,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="36" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -27140,7 +26240,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -27171,1276 +26271,756 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="B4" s="3">
-        <v>6706873292.2517996</v>
+        <v>66442468040.323997</v>
       </c>
       <c r="C4" s="3">
-        <v>130869362668.7</v>
+        <v>472689604063.90002</v>
       </c>
       <c r="D4" s="3">
-        <v>3681719617.8639998</v>
+        <v>244410080985.98001</v>
       </c>
       <c r="E4" s="3">
-        <v>8726084495.9743996</v>
+        <v>120208506407.52</v>
       </c>
       <c r="F4" s="3">
-        <v>7601603928.4404001</v>
+        <v>138870979271.69</v>
       </c>
       <c r="G4" s="3">
-        <v>3637367998.9530001</v>
+        <v>138311918804.81</v>
       </c>
       <c r="H4" s="3">
-        <v>40225319701.610001</v>
+        <v>302048246050.73999</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>1971</v>
+        <v>1991</v>
       </c>
       <c r="B5" s="3">
-        <v>6664236463.7439003</v>
+        <v>63980718012.218002</v>
       </c>
       <c r="C5" s="3">
-        <v>151066079936.64999</v>
+        <v>445748690065.41998</v>
       </c>
       <c r="D5" s="3">
-        <v>4275664365.8361001</v>
+        <v>230483190942.89001</v>
       </c>
       <c r="E5" s="3">
-        <v>9567596236.1576004</v>
+        <v>105787427091.14999</v>
       </c>
       <c r="F5" s="3">
-        <v>9104786453.3546009</v>
+        <v>134178717570.94</v>
       </c>
       <c r="G5" s="3">
-        <v>4108961583.9742999</v>
+        <v>130339108450.56</v>
       </c>
       <c r="H5" s="3">
-        <v>45908857962.728996</v>
+        <v>304856274888.58002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>1972</v>
+        <v>1992</v>
       </c>
       <c r="B6" s="3">
-        <v>7565752327.9068003</v>
+        <v>58222866436.445999</v>
       </c>
       <c r="C6" s="3">
-        <v>171573485728.35001</v>
+        <v>365915592345.45001</v>
       </c>
       <c r="D6" s="3">
-        <v>4996882988.3734999</v>
+        <v>189201173921.89001</v>
       </c>
       <c r="E6" s="3">
-        <v>10213449415.110001</v>
+        <v>70876590787.927994</v>
       </c>
       <c r="F6" s="3">
-        <v>12313009899.584</v>
+        <v>127705302371.55</v>
       </c>
       <c r="G6" s="3">
-        <v>5977509748.3056002</v>
+        <v>109377229559.28999</v>
       </c>
       <c r="H6" s="3">
-        <v>52922190211.123001</v>
+        <v>287262862205.26001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>1973</v>
+        <v>1993</v>
       </c>
       <c r="B7" s="3">
-        <v>8004462821.2784004</v>
+        <v>55893956971.064003</v>
       </c>
       <c r="C7" s="3">
-        <v>189838035760.06</v>
+        <v>313107191782.65997</v>
       </c>
       <c r="D7" s="3">
-        <v>5913623795.026</v>
+        <v>161893772033</v>
       </c>
       <c r="E7" s="3">
-        <v>13877912922.976999</v>
+        <v>65206446180.060997</v>
       </c>
       <c r="F7" s="3">
-        <v>10919719300.884001</v>
+        <v>123746451395.02</v>
       </c>
       <c r="G7" s="3">
-        <v>7074240647.9315996</v>
+        <v>87343204484.615997</v>
       </c>
       <c r="H7" s="3">
-        <v>54714940452.987</v>
+        <v>292458199671.38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>1974</v>
+        <v>1994</v>
       </c>
       <c r="B8" s="3">
-        <v>8279435516.0474997</v>
+        <v>49295163815.666</v>
       </c>
       <c r="C8" s="3">
-        <v>190709422649.79999</v>
+        <v>250375859544.44</v>
       </c>
       <c r="D8" s="3">
-        <v>6877400598.8006001</v>
+        <v>129467269908.39</v>
       </c>
       <c r="E8" s="3">
-        <v>15110377374.108999</v>
+        <v>52817228107.271004</v>
       </c>
       <c r="F8" s="3">
-        <v>13351248562.684999</v>
+        <v>123622698881.08</v>
       </c>
       <c r="G8" s="3">
-        <v>9453922820.1963997</v>
+        <v>73272571212.809998</v>
       </c>
       <c r="H8" s="3">
-        <v>79265027120.636993</v>
+        <v>262983800484</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>1975</v>
+        <v>1995</v>
       </c>
       <c r="B9" s="3">
-        <v>9094086150.7007999</v>
+        <v>44514811692.658997</v>
       </c>
       <c r="C9" s="3">
-        <v>169378552430.70001</v>
+        <v>241515372824.42001</v>
       </c>
       <c r="D9" s="3">
-        <v>7440910289.8113003</v>
+        <v>124873094669.96001</v>
       </c>
       <c r="E9" s="3">
-        <v>16866943563.929001</v>
+        <v>48063679154.410004</v>
       </c>
       <c r="F9" s="3">
-        <v>16753016292.819</v>
+        <v>118554187644.11</v>
       </c>
       <c r="G9" s="3">
-        <v>11501013469.243</v>
+        <v>71413488571.852005</v>
       </c>
       <c r="H9" s="3">
-        <v>91758968546.654999</v>
+        <v>257192222909.42999</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>1976</v>
+        <v>1996</v>
       </c>
       <c r="B10" s="3">
-        <v>10160101394.666</v>
+        <v>42215957228.322998</v>
       </c>
       <c r="C10" s="3">
-        <v>192630258142.47</v>
+        <v>234944190934.87</v>
       </c>
       <c r="D10" s="3">
-        <v>9675581290.3334999</v>
+        <v>121474291431.78999</v>
       </c>
       <c r="E10" s="3">
-        <v>28899671977.523998</v>
+        <v>39993840931.055</v>
       </c>
       <c r="F10" s="3">
-        <v>19466987563.068001</v>
+        <v>120978939301.61</v>
       </c>
       <c r="G10" s="3">
-        <v>12162589171.452</v>
+        <v>68082061692.324997</v>
       </c>
       <c r="H10" s="3">
-        <v>104488629523.25</v>
+        <v>258981072463.39001</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>1977</v>
+        <v>1997</v>
       </c>
       <c r="B11" s="3">
-        <v>9762577513.1532001</v>
+        <v>42936704451.253998</v>
       </c>
       <c r="C11" s="3">
-        <v>178637697264.97</v>
+        <v>239195246942.70001</v>
       </c>
       <c r="D11" s="3">
-        <v>10157008554.993999</v>
+        <v>123711873318.17</v>
       </c>
       <c r="E11" s="3">
-        <v>23488383409.096001</v>
+        <v>37818812404.108002</v>
       </c>
       <c r="F11" s="3">
-        <v>18576602489.641998</v>
+        <v>127447024761.91</v>
       </c>
       <c r="G11" s="3">
-        <v>12273055315.690001</v>
+        <v>66848215964.595001</v>
       </c>
       <c r="H11" s="3">
-        <v>112249701910.16</v>
+        <v>262048918509.98001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>1978</v>
+        <v>1998</v>
       </c>
       <c r="B12" s="3">
-        <v>10415509120.032</v>
+        <v>35086807903.407997</v>
       </c>
       <c r="C12" s="3">
-        <v>129411124067.77</v>
+        <v>227256022870.07999</v>
       </c>
       <c r="D12" s="3">
-        <v>9095470659.1620007</v>
+        <v>117465179459.12</v>
       </c>
       <c r="E12" s="3">
-        <v>29283239963.227001</v>
+        <v>35437867065.652</v>
       </c>
       <c r="F12" s="3">
-        <v>19030312004.263</v>
+        <v>119302300380.28</v>
       </c>
       <c r="G12" s="3">
-        <v>11417356770.43</v>
+        <v>64918823354.265999</v>
       </c>
       <c r="H12" s="3">
-        <v>118394669901.39999</v>
+        <v>261875364882.35999</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>1979</v>
+        <v>1999</v>
       </c>
       <c r="B13" s="3">
-        <v>11047500636.572001</v>
+        <v>40803806293.120003</v>
       </c>
       <c r="C13" s="3">
-        <v>101874260383.45</v>
+        <v>249766862085.98001</v>
       </c>
       <c r="D13" s="3">
-        <v>7923259828.9252996</v>
+        <v>129134172445.12</v>
       </c>
       <c r="E13" s="3">
-        <v>22513342054.650002</v>
+        <v>37546780242.907997</v>
       </c>
       <c r="F13" s="3">
-        <v>16823783003.447001</v>
+        <v>117008165851.37</v>
       </c>
       <c r="G13" s="3">
-        <v>12505244763.973</v>
+        <v>71107805680.613007</v>
       </c>
       <c r="H13" s="3">
-        <v>127491074116.66</v>
+        <v>269753960628.45001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>1980</v>
+        <v>2000</v>
       </c>
       <c r="B14" s="3">
-        <v>11454716518.083</v>
+        <v>45720146034.627998</v>
       </c>
       <c r="C14" s="3">
-        <v>40370031993.899002</v>
+        <v>277715907823.65997</v>
       </c>
       <c r="D14" s="3">
-        <v>8898103926.1403008</v>
+        <v>143772840067.81</v>
       </c>
       <c r="E14" s="3">
-        <v>22015522625.543999</v>
+        <v>44076146673.744003</v>
       </c>
       <c r="F14" s="3">
-        <v>14597828004.705</v>
+        <v>131265839803.42999</v>
       </c>
       <c r="G14" s="3">
-        <v>12679758813.695999</v>
+        <v>75485396546.813004</v>
       </c>
       <c r="H14" s="3">
-        <v>122777513770.83</v>
+        <v>276320916932.79999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>1981</v>
+        <v>2001</v>
       </c>
       <c r="B15" s="3">
-        <v>11666808115.281</v>
+        <v>50776369593.107002</v>
       </c>
       <c r="C15" s="3">
-        <v>43445828678.880997</v>
+        <v>291077805139.98999</v>
       </c>
       <c r="D15" s="3">
-        <v>9612866627.5041008</v>
+        <v>150178092612.64999</v>
       </c>
       <c r="E15" s="3">
-        <v>17843013160.507999</v>
+        <v>48439690014.873001</v>
       </c>
       <c r="F15" s="3">
-        <v>13605829203.864</v>
+        <v>136430896030.75</v>
       </c>
       <c r="G15" s="3">
-        <v>10329174013.35</v>
+        <v>79697833873.326996</v>
       </c>
       <c r="H15" s="3">
-        <v>110394567110.81</v>
+        <v>282234065363.02002</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>1982</v>
+        <v>2002</v>
       </c>
       <c r="B16" s="3">
-        <v>12497595052.781</v>
+        <v>52250290430.009003</v>
       </c>
       <c r="C16" s="3">
-        <v>84887644321.947006</v>
+        <v>302191738520.89001</v>
       </c>
       <c r="D16" s="3">
-        <v>9192309476.7660999</v>
+        <v>156360353117.95001</v>
       </c>
       <c r="E16" s="3">
-        <v>19860970867.632999</v>
+        <v>49795994099.521004</v>
       </c>
       <c r="F16" s="3">
-        <v>13967818868.943001</v>
+        <v>147614942968.70001</v>
       </c>
       <c r="G16" s="3">
-        <v>10804024033.627001</v>
+        <v>84245602008.166</v>
       </c>
       <c r="H16" s="3">
-        <v>105510878649.14999</v>
+        <v>290275229810.28003</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>1983</v>
+        <v>2003</v>
       </c>
       <c r="B17" s="3">
-        <v>13066657984.997</v>
+        <v>51459651854.557999</v>
       </c>
       <c r="C17" s="3">
-        <v>87401817783.488998</v>
+        <v>327319754016.82001</v>
       </c>
       <c r="D17" s="3">
-        <v>10286126978.466</v>
+        <v>170119080064.41</v>
       </c>
       <c r="E17" s="3">
-        <v>24351196082.709999</v>
+        <v>56097983872.718002</v>
       </c>
       <c r="F17" s="3">
-        <v>19922731600.384998</v>
+        <v>166571619299.01001</v>
       </c>
       <c r="G17" s="3">
-        <v>12487165933.76</v>
+        <v>90351992200.259995</v>
       </c>
       <c r="H17" s="3">
-        <v>104518243763.2</v>
+        <v>300096376842.32001</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>1984</v>
+        <v>2004</v>
       </c>
       <c r="B18" s="3">
-        <v>14025818301.837999</v>
+        <v>52054778985.733002</v>
       </c>
       <c r="C18" s="3">
-        <v>73621880277.098007</v>
+        <v>359962969062.09998</v>
       </c>
       <c r="D18" s="3">
-        <v>11549642979.587</v>
+        <v>183818435630.41</v>
       </c>
       <c r="E18" s="3">
-        <v>19697622719.338001</v>
+        <v>61648136967.953003</v>
       </c>
       <c r="F18" s="3">
-        <v>22872423665.710999</v>
+        <v>183267914028.20001</v>
       </c>
       <c r="G18" s="3">
-        <v>12721152035.978001</v>
+        <v>95688374675.820999</v>
       </c>
       <c r="H18" s="3">
-        <v>97512747365.591995</v>
+        <v>306524184779.96002</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>1985</v>
+        <v>2005</v>
       </c>
       <c r="B19" s="3">
-        <v>15133629918.379999</v>
+        <v>51799979961.103996</v>
       </c>
       <c r="C19" s="3">
-        <v>74708834434.481003</v>
+        <v>370203498365.26001</v>
       </c>
       <c r="D19" s="3">
-        <v>11306162523.896</v>
+        <v>191974881733.48001</v>
       </c>
       <c r="E19" s="3">
-        <v>18142148653.493999</v>
+        <v>67944479297.449997</v>
       </c>
       <c r="F19" s="3">
-        <v>21763426612</v>
+        <v>200034461372.57001</v>
       </c>
       <c r="G19" s="3">
-        <v>12729910723.907</v>
+        <v>101352116760.17999</v>
       </c>
       <c r="H19" s="3">
-        <v>102970708559.57001</v>
+        <v>324692050255.54999</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>1986</v>
+        <v>2006</v>
       </c>
       <c r="B20" s="3">
-        <v>15853140799.039</v>
+        <v>53248749121.992996</v>
       </c>
       <c r="C20" s="3">
-        <v>65952793048.623001</v>
+        <v>380397538207.01001</v>
       </c>
       <c r="D20" s="3">
-        <v>10587710724.719</v>
+        <v>204591607128.85001</v>
       </c>
       <c r="E20" s="3">
-        <v>20605246319.488998</v>
+        <v>76621861523.875</v>
       </c>
       <c r="F20" s="3">
-        <v>19418524832.323002</v>
+        <v>227714516562.48999</v>
       </c>
       <c r="G20" s="3">
-        <v>11025559885.535</v>
+        <v>111207460124.37</v>
       </c>
       <c r="H20" s="3">
-        <v>86676187228.852997</v>
+        <v>350601290430.21997</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>1987</v>
+        <v>2007</v>
       </c>
       <c r="B21" s="3">
-        <v>16246829838.121</v>
+        <v>53884648662.874001</v>
       </c>
       <c r="C21" s="3">
-        <v>75010824596.966995</v>
+        <v>390286837986.44</v>
       </c>
       <c r="D21" s="3">
-        <v>11764532927.223</v>
+        <v>219981762251.89999</v>
       </c>
       <c r="E21" s="3">
-        <v>19452878302.650002</v>
+        <v>86588899388.774002</v>
       </c>
       <c r="F21" s="3">
-        <v>19356561824.5</v>
+        <v>254574139947.89999</v>
       </c>
       <c r="G21" s="3">
-        <v>9023554021.1506996</v>
+        <v>116594715069.25999</v>
       </c>
       <c r="H21" s="3">
-        <v>78228615550.632004</v>
+        <v>396538405306.84003</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>1988</v>
+        <v>2008</v>
       </c>
       <c r="B22" s="3">
-        <v>16142503388.804001</v>
+        <v>57006184227.819</v>
       </c>
       <c r="C22" s="3">
-        <v>80091520051.707993</v>
+        <v>387482512094.17999</v>
       </c>
       <c r="D22" s="3">
-        <v>12006168834.006001</v>
+        <v>215313223774.62</v>
       </c>
       <c r="E22" s="3">
-        <v>12777456062.875</v>
+        <v>96177536374.621002</v>
       </c>
       <c r="F22" s="3">
-        <v>18730113088.596001</v>
+        <v>279706029031.77002</v>
       </c>
       <c r="G22" s="3">
-        <v>8417351754.6497002</v>
+        <v>122705903050.72</v>
       </c>
       <c r="H22" s="3">
-        <v>66711191333.992996</v>
+        <v>424386984462.5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>1989</v>
+        <v>2009</v>
       </c>
       <c r="B23" s="3">
-        <v>16842521804.372999</v>
+        <v>57945664001.514999</v>
       </c>
       <c r="C23" s="3">
-        <v>85062716858.738007</v>
+        <v>352138362390.67999</v>
       </c>
       <c r="D23" s="3">
-        <v>12432324839.715</v>
+        <v>183843231426.53</v>
       </c>
       <c r="E23" s="3">
-        <v>12717873330.231001</v>
+        <v>82037511049.380997</v>
       </c>
       <c r="F23" s="3">
-        <v>20374859395.463001</v>
+        <v>262143312785.73999</v>
       </c>
       <c r="G23" s="3">
-        <v>9280262238.3185997</v>
+        <v>112183029691.75</v>
       </c>
       <c r="H23" s="3">
-        <v>70113675035.927994</v>
+        <v>412578856136.28003</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>1990</v>
+        <v>2010</v>
       </c>
       <c r="B24" s="3">
-        <v>18700051593.625</v>
+        <v>51004299298.551003</v>
       </c>
       <c r="C24" s="3">
-        <v>102317396486.14999</v>
+        <v>377688222229.25</v>
       </c>
       <c r="D24" s="3">
-        <v>15928841990.087999</v>
+        <v>199669508795.01001</v>
       </c>
       <c r="E24" s="3">
-        <v>13102966279.813</v>
+        <v>85673914628.449005</v>
       </c>
       <c r="F24" s="3">
-        <v>21710330971.335999</v>
+        <v>277439640369.34003</v>
       </c>
       <c r="G24" s="3">
-        <v>10143891208.299</v>
+        <v>118329718079.89999</v>
       </c>
       <c r="H24" s="3">
-        <v>77622235255.556</v>
+        <v>422278449043.40002</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>1991</v>
+        <v>2011</v>
       </c>
       <c r="B25" s="3">
-        <v>19750810853.791</v>
+        <v>58180627642.765999</v>
       </c>
       <c r="C25" s="3">
-        <v>116965914532.11</v>
+        <v>394282114694.96002</v>
       </c>
       <c r="D25" s="3">
-        <v>19303859407.09</v>
+        <v>212213416439.89001</v>
       </c>
       <c r="E25" s="3">
-        <v>16945338972.913</v>
+        <v>92222350752.942993</v>
       </c>
       <c r="F25" s="3">
-        <v>24414353220.534</v>
+        <v>286733472500.53998</v>
       </c>
       <c r="G25" s="3">
-        <v>10290708658.847</v>
+        <v>125983276335.22</v>
       </c>
       <c r="H25" s="3">
-        <v>85335594342.412994</v>
+        <v>425820046232.83002</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>1992</v>
+        <v>2012</v>
       </c>
       <c r="B26" s="3">
-        <v>21782327889.522999</v>
+        <v>57484959421.547997</v>
       </c>
       <c r="C26" s="3">
-        <v>117688256239.27</v>
+        <v>406528942968.38</v>
       </c>
       <c r="D26" s="3">
-        <v>19127970072.530998</v>
+        <v>221902498582.56</v>
       </c>
       <c r="E26" s="3">
-        <v>17890497335.757999</v>
+        <v>95757707353.110992</v>
       </c>
       <c r="F26" s="3">
-        <v>26010424933.701</v>
+        <v>296787766017.81</v>
       </c>
       <c r="G26" s="3">
-        <v>10567515528.224001</v>
+        <v>131017664115.81</v>
       </c>
       <c r="H26" s="3">
-        <v>87848056784.927994</v>
+        <v>445516678133.90002</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>1993</v>
+        <v>2013</v>
       </c>
       <c r="B27" s="3">
-        <v>21992260805.82</v>
+        <v>60087433894.948997</v>
       </c>
       <c r="C27" s="3">
-        <v>122425085663.24001</v>
+        <v>406991912729.28003</v>
       </c>
       <c r="D27" s="3">
-        <v>18126387835.278</v>
+        <v>223483559630.35999</v>
       </c>
       <c r="E27" s="3">
-        <v>17917384274.603001</v>
+        <v>94279204003.546005</v>
       </c>
       <c r="F27" s="3">
-        <v>24203137590.994999</v>
+        <v>297014474557.53998</v>
       </c>
       <c r="G27" s="3">
-        <v>12343139898.517</v>
+        <v>130777232909.61</v>
       </c>
       <c r="H27" s="3">
-        <v>89777048759.035004</v>
+        <v>466887563323.01001</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>1994</v>
+        <v>2014</v>
       </c>
       <c r="B28" s="3">
-        <v>22456588252.125999</v>
+        <v>60998034780.926003</v>
       </c>
       <c r="C28" s="3">
-        <v>118009034674.74001</v>
+        <v>408178729802.64001</v>
       </c>
       <c r="D28" s="3">
-        <v>18729448809.678001</v>
+        <v>225159739561.07999</v>
       </c>
       <c r="E28" s="3">
-        <v>17670310296.113998</v>
+        <v>94042783671.820999</v>
       </c>
       <c r="F28" s="3">
-        <v>23373337186.005001</v>
+        <v>306893856324.32001</v>
       </c>
       <c r="G28" s="3">
-        <v>13614175277.226999</v>
+        <v>135148628829.33</v>
       </c>
       <c r="H28" s="3">
-        <v>92359548579.569</v>
+        <v>466119863669.54999</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>1995</v>
+        <v>2015</v>
       </c>
       <c r="B29" s="3">
-        <v>23289320118.015999</v>
+        <v>62754805353.154999</v>
       </c>
       <c r="C29" s="3">
-        <v>119755174269.34</v>
+        <v>396458190565.85999</v>
       </c>
       <c r="D29" s="3">
-        <v>18727221492.556999</v>
+        <v>214740225530.82999</v>
       </c>
       <c r="E29" s="3">
-        <v>16541373499.302</v>
+        <v>93500769315.306</v>
       </c>
       <c r="F29" s="3">
-        <v>23157068739.518002</v>
+        <v>297855130196.84003</v>
       </c>
       <c r="G29" s="3">
-        <v>14995295525.047001</v>
+        <v>131269445323.8</v>
       </c>
       <c r="H29" s="3">
-        <v>94544695875.408997</v>
+        <v>455804039892.94</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>1996</v>
+        <v>2016</v>
       </c>
       <c r="B30" s="3">
-        <v>22818443161.257</v>
+        <v>64843098747.899002</v>
       </c>
       <c r="C30" s="3">
-        <v>121664429935.45</v>
+        <v>397044320119.84003</v>
       </c>
       <c r="D30" s="3">
-        <v>21436323507.366001</v>
+        <v>217206986056.67001</v>
       </c>
       <c r="E30" s="3">
-        <v>18543152041.021</v>
+        <v>92435140348.725006</v>
       </c>
       <c r="F30" s="3">
-        <v>27016329930.327999</v>
+        <v>295124767825.01001</v>
       </c>
       <c r="G30" s="3">
-        <v>17117711323.284</v>
+        <v>129992581888.71001</v>
       </c>
       <c r="H30" s="3">
-        <v>90663712369.509003</v>
+        <v>454537198358.35999</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>1997</v>
+        <v>2017</v>
       </c>
       <c r="B31" s="3">
-        <v>22168065968.299</v>
+        <v>65616047808.931</v>
       </c>
       <c r="C31" s="3">
-        <v>120357940237.16</v>
+        <v>398920728220.5</v>
       </c>
       <c r="D31" s="3">
-        <v>24378158925.900002</v>
+        <v>217402467511.79001</v>
       </c>
       <c r="E31" s="3">
-        <v>15778984005.614</v>
+        <v>93282461233.804001</v>
       </c>
       <c r="F31" s="3">
-        <v>27782377957.234001</v>
+        <v>302564293485.40997</v>
       </c>
       <c r="G31" s="3">
-        <v>17458898678.555</v>
+        <v>133285382801.49001</v>
       </c>
       <c r="H31" s="3">
-        <v>95000099341.766006</v>
+        <v>462840969890.66998</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
-        <v>1998</v>
+      <c r="A32" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B32" s="3">
-        <v>24712972224.577</v>
+        <v>1506509030666.5471</v>
       </c>
       <c r="C32" s="3">
-        <v>122113168268.84</v>
+        <v>9665384718397.6582</v>
       </c>
       <c r="D32" s="3">
-        <v>23516239059.049</v>
+        <v>5123846009033.1094</v>
       </c>
       <c r="E32" s="3">
-        <v>14368083217.231001</v>
+        <v>2024379748942.6782</v>
       </c>
       <c r="F32" s="3">
-        <v>28866204659.923</v>
+        <v>5601151840536.9297</v>
       </c>
       <c r="G32" s="3">
-        <v>17969193311.271999</v>
+        <v>2906330782060.2734</v>
       </c>
       <c r="H32" s="3">
-        <v>96634635397.994003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
-        <v>1999</v>
-      </c>
-      <c r="B33" s="3">
-        <v>23351032499.226002</v>
-      </c>
-      <c r="C33" s="3">
-        <v>119652667423.75</v>
-      </c>
-      <c r="D33" s="3">
-        <v>25973246221.300999</v>
-      </c>
-      <c r="E33" s="3">
-        <v>17378782558.362</v>
-      </c>
-      <c r="F33" s="3">
-        <v>29223060271.693001</v>
-      </c>
-      <c r="G33" s="3">
-        <v>20441646070.469002</v>
-      </c>
-      <c r="H33" s="3">
-        <v>97913097875.828003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
-        <v>2000</v>
-      </c>
-      <c r="B34" s="3">
-        <v>24255768993.848999</v>
-      </c>
-      <c r="C34" s="3">
-        <v>130216122049.99001</v>
-      </c>
-      <c r="D34" s="3">
-        <v>28961106686.272999</v>
-      </c>
-      <c r="E34" s="3">
-        <v>18798214805.714001</v>
-      </c>
-      <c r="F34" s="3">
-        <v>30957156988.033001</v>
-      </c>
-      <c r="G34" s="3">
-        <v>21543621547.629002</v>
-      </c>
-      <c r="H34" s="3">
-        <v>97961614915.186996</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
-        <v>2001</v>
-      </c>
-      <c r="B35" s="3">
-        <v>23647756556.93</v>
-      </c>
-      <c r="C35" s="3">
-        <v>123393065487.36</v>
-      </c>
-      <c r="D35" s="3">
-        <v>32473612459.000999</v>
-      </c>
-      <c r="E35" s="3">
-        <v>21784860540.119999</v>
-      </c>
-      <c r="F35" s="3">
-        <v>33610506477.310001</v>
-      </c>
-      <c r="G35" s="3">
-        <v>22960017997.910999</v>
-      </c>
-      <c r="H35" s="3">
-        <v>101404774965.24001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
-        <v>2002</v>
-      </c>
-      <c r="B36" s="3">
-        <v>27043184943.029999</v>
-      </c>
-      <c r="C36" s="3">
-        <v>130797047476.2</v>
-      </c>
-      <c r="D36" s="3">
-        <v>36793202261.731003</v>
-      </c>
-      <c r="E36" s="3">
-        <v>26280484467.533001</v>
-      </c>
-      <c r="F36" s="3">
-        <v>36312507285.532997</v>
-      </c>
-      <c r="G36" s="3">
-        <v>24306456479.300999</v>
-      </c>
-      <c r="H36" s="3">
-        <v>107883664846.96001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
-        <v>2003</v>
-      </c>
-      <c r="B37" s="3">
-        <v>28809288119.507999</v>
-      </c>
-      <c r="C37" s="3">
-        <v>147227540327.5</v>
-      </c>
-      <c r="D37" s="3">
-        <v>40381954667.922997</v>
-      </c>
-      <c r="E37" s="3">
-        <v>26044312518.067001</v>
-      </c>
-      <c r="F37" s="3">
-        <v>39831520283.874001</v>
-      </c>
-      <c r="G37" s="3">
-        <v>28838645423.532001</v>
-      </c>
-      <c r="H37" s="3">
-        <v>110348628264.67999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
-        <v>2004</v>
-      </c>
-      <c r="B38" s="3">
-        <v>28507940776.832001</v>
-      </c>
-      <c r="C38" s="3">
-        <v>152148018407.07999</v>
-      </c>
-      <c r="D38" s="3">
-        <v>41907390030.185997</v>
-      </c>
-      <c r="E38" s="3">
-        <v>26061352650.664001</v>
-      </c>
-      <c r="F38" s="3">
-        <v>44331626483.068001</v>
-      </c>
-      <c r="G38" s="3">
-        <v>31307076058.085999</v>
-      </c>
-      <c r="H38" s="3">
-        <v>114845850049.77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
-        <v>2005</v>
-      </c>
-      <c r="B39" s="3">
-        <v>31862757398.654999</v>
-      </c>
-      <c r="C39" s="3">
-        <v>156656490758.73999</v>
-      </c>
-      <c r="D39" s="3">
-        <v>46309416806.348999</v>
-      </c>
-      <c r="E39" s="3">
-        <v>26735374735.150002</v>
-      </c>
-      <c r="F39" s="3">
-        <v>48236277298.360001</v>
-      </c>
-      <c r="G39" s="3">
-        <v>33696064528.417</v>
-      </c>
-      <c r="H39" s="3">
-        <v>122199102065.78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
-        <v>2006</v>
-      </c>
-      <c r="B40" s="3">
-        <v>34328899942.133999</v>
-      </c>
-      <c r="C40" s="3">
-        <v>164353668794.04001</v>
-      </c>
-      <c r="D40" s="3">
-        <v>49980505769.668999</v>
-      </c>
-      <c r="E40" s="3">
-        <v>25933872763.188999</v>
-      </c>
-      <c r="F40" s="3">
-        <v>50168783512.267998</v>
-      </c>
-      <c r="G40" s="3">
-        <v>36794303384.941002</v>
-      </c>
-      <c r="H40" s="3">
-        <v>131992755410.60001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
-        <v>2007</v>
-      </c>
-      <c r="B41" s="3">
-        <v>35091485243.765999</v>
-      </c>
-      <c r="C41" s="3">
-        <v>168052911727.89999</v>
-      </c>
-      <c r="D41" s="3">
-        <v>50968211138.001999</v>
-      </c>
-      <c r="E41" s="3">
-        <v>32392031992.330002</v>
-      </c>
-      <c r="F41" s="3">
-        <v>53392765615.635002</v>
-      </c>
-      <c r="G41" s="3">
-        <v>40546640112.466003</v>
-      </c>
-      <c r="H41" s="3">
-        <v>145172866525.81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
-        <v>2008</v>
-      </c>
-      <c r="B42" s="3">
-        <v>27949235421.088001</v>
-      </c>
-      <c r="C42" s="3">
-        <v>169828801821.12</v>
-      </c>
-      <c r="D42" s="3">
-        <v>52556105253.031998</v>
-      </c>
-      <c r="E42" s="3">
-        <v>36573667508.332001</v>
-      </c>
-      <c r="F42" s="3">
-        <v>51025727698.656998</v>
-      </c>
-      <c r="G42" s="3">
-        <v>44340960941.999001</v>
-      </c>
-      <c r="H42" s="3">
-        <v>140947416923.17001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
-        <v>2009</v>
-      </c>
-      <c r="B43" s="3">
-        <v>30078539446.521</v>
-      </c>
-      <c r="C43" s="3">
-        <v>169742495883.82999</v>
-      </c>
-      <c r="D43" s="3">
-        <v>56816724302.574997</v>
-      </c>
-      <c r="E43" s="3">
-        <v>34835208456.039001</v>
-      </c>
-      <c r="F43" s="3">
-        <v>53388893157.902</v>
-      </c>
-      <c r="G43" s="3">
-        <v>47516688169.103996</v>
-      </c>
-      <c r="H43" s="3">
-        <v>137675037259.76999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
-        <v>2010</v>
-      </c>
-      <c r="B44" s="3">
-        <v>31918418894.811001</v>
-      </c>
-      <c r="C44" s="3">
-        <v>181572240871.29001</v>
-      </c>
-      <c r="D44" s="3">
-        <v>62781599464.891998</v>
-      </c>
-      <c r="E44" s="3">
-        <v>35539431280.113998</v>
-      </c>
-      <c r="F44" s="3">
-        <v>57236483271.041</v>
-      </c>
-      <c r="G44" s="3">
-        <v>50071734330.658997</v>
-      </c>
-      <c r="H44" s="3">
-        <v>143826440306.85999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
-        <v>2011</v>
-      </c>
-      <c r="B45" s="3">
-        <v>33106636958.527</v>
-      </c>
-      <c r="C45" s="3">
-        <v>183846079410.39999</v>
-      </c>
-      <c r="D45" s="3">
-        <v>66327162530.347</v>
-      </c>
-      <c r="E45" s="3">
-        <v>37347333486.434998</v>
-      </c>
-      <c r="F45" s="3">
-        <v>59447581734.342003</v>
-      </c>
-      <c r="G45" s="3">
-        <v>51464646284.294998</v>
-      </c>
-      <c r="H45" s="3">
-        <v>150338525088.13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B46" s="3">
-        <v>34649110324.593002</v>
-      </c>
-      <c r="C46" s="3">
-        <v>145820599118.47</v>
-      </c>
-      <c r="D46" s="3">
-        <v>63623361867.805</v>
-      </c>
-      <c r="E46" s="3">
-        <v>36142951484.542999</v>
-      </c>
-      <c r="F46" s="3">
-        <v>54562270321.863998</v>
-      </c>
-      <c r="G46" s="3">
-        <v>54431392359.763</v>
-      </c>
-      <c r="H46" s="3">
-        <v>157064156080.22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="2">
-        <v>2013</v>
-      </c>
-      <c r="B47" s="3">
-        <v>36547017215.188004</v>
-      </c>
-      <c r="C47" s="3">
-        <v>140814434654.04001</v>
-      </c>
-      <c r="D47" s="3">
-        <v>60282351660.946999</v>
-      </c>
-      <c r="E47" s="3">
-        <v>32801140731.603001</v>
-      </c>
-      <c r="F47" s="3">
-        <v>54356633078.899002</v>
-      </c>
-      <c r="G47" s="3">
-        <v>54953414699.585999</v>
-      </c>
-      <c r="H47" s="3">
-        <v>163033208188.29999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
-        <v>2014</v>
-      </c>
-      <c r="B48" s="3">
-        <v>38523380400.382004</v>
-      </c>
-      <c r="C48" s="3">
-        <v>149861413054.53</v>
-      </c>
-      <c r="D48" s="3">
-        <v>65096974759.447998</v>
-      </c>
-      <c r="E48" s="3">
-        <v>32501474897.666</v>
-      </c>
-      <c r="F48" s="3">
-        <v>54624034899.174004</v>
-      </c>
-      <c r="G48" s="3">
-        <v>55812510146.769997</v>
-      </c>
-      <c r="H48" s="3">
-        <v>165873074327.03</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
-        <v>2015</v>
-      </c>
-      <c r="B49" s="3">
-        <v>40304054184.188004</v>
-      </c>
-      <c r="C49" s="3">
-        <v>152391762722.35001</v>
-      </c>
-      <c r="D49" s="3">
-        <v>62076760507.538002</v>
-      </c>
-      <c r="E49" s="3">
-        <v>26974113590.859001</v>
-      </c>
-      <c r="F49" s="3">
-        <v>51300514902.539001</v>
-      </c>
-      <c r="G49" s="3">
-        <v>52421356725.643997</v>
-      </c>
-      <c r="H49" s="3">
-        <v>166580315082.38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
-        <v>2016</v>
-      </c>
-      <c r="B50" s="3">
-        <v>41995259096.741997</v>
-      </c>
-      <c r="C50" s="3">
-        <v>199427095834.62</v>
-      </c>
-      <c r="D50" s="3">
-        <v>66333642656.197998</v>
-      </c>
-      <c r="E50" s="3">
-        <v>23451245231.005001</v>
-      </c>
-      <c r="F50" s="3">
-        <v>54494992922.711998</v>
-      </c>
-      <c r="G50" s="3">
-        <v>55914526209.014</v>
-      </c>
-      <c r="H50" s="3">
-        <v>169334026580.57001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B51" s="3">
-        <v>43329852262.586998</v>
-      </c>
-      <c r="C51" s="3">
-        <v>205884468894.5</v>
-      </c>
-      <c r="D51" s="3">
-        <v>69855332020.781006</v>
-      </c>
-      <c r="E51" s="3">
-        <v>23728986935.409</v>
-      </c>
-      <c r="F51" s="3">
-        <v>57077832347.925003</v>
-      </c>
-      <c r="G51" s="3">
-        <v>59862466928.68</v>
-      </c>
-      <c r="H51" s="3">
-        <v>175066490614.57001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="3">
-        <v>1043601216503.6405</v>
-      </c>
-      <c r="C52" s="3">
-        <v>6369525496102.7617</v>
-      </c>
-      <c r="D52" s="3">
-        <v>1336446583990.6838</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1056073860092.7294</v>
-      </c>
-      <c r="F52" s="3">
-        <v>1468663920335.0798</v>
-      </c>
-      <c r="G52" s="3">
-        <v>1111333873551.6592</v>
-      </c>
-      <c r="H52" s="3">
-        <v>5182080379892.8047</v>
+        <v>9723514091558</v>
       </c>
     </row>
   </sheetData>
@@ -28454,7 +27034,7 @@
   <dimension ref="A1:I1965"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>